<commit_message>
création de scripts d'exploration + analyse des données pour future sélection
</commit_message>
<xml_diff>
--- a/Admin/Dashboard_Appli_BI.xlsx
+++ b/Admin/Dashboard_Appli_BI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexi\Documents\files\Cours\Master\S9\UE_appli_bi\BanqueBI\Admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823CF25B-B78D-44C8-8D11-09D9FEA09589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0045978-B16C-4ADE-AFE2-FABE58046EA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="42">
   <si>
     <t>Tâches</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Rapport</t>
   </si>
   <si>
-    <t>Projet</t>
-  </si>
-  <si>
     <t>Courte description des jeux de données</t>
   </si>
   <si>
@@ -151,6 +148,9 @@
   </si>
   <si>
     <t>Abdelghani</t>
+  </si>
+  <si>
+    <t>Python / Anaconda / VSC</t>
   </si>
 </sst>
 </file>
@@ -943,440 +943,446 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:H33"/>
+  <dimension ref="B1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="17.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="82.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="32.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="2" customWidth="1"/>
-    <col min="6" max="7" width="20.7109375" style="27" customWidth="1"/>
-    <col min="8" max="8" width="27.5703125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="82.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="32.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="2" customWidth="1"/>
+    <col min="5" max="6" width="20.7109375" style="27" customWidth="1"/>
+    <col min="7" max="7" width="55.5703125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E1" s="1"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="2:8" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="2:7" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="41" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="32">
+        <v>45565</v>
+      </c>
+      <c r="F4" s="33"/>
+      <c r="G4" s="42"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="41" t="s">
+      <c r="C5" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="24">
+        <v>45565</v>
+      </c>
+      <c r="F5" s="34">
+        <v>45565</v>
+      </c>
+      <c r="G5" s="11"/>
+    </row>
+    <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="9" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="15" t="s">
+      <c r="C6" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="25">
+        <v>45565</v>
+      </c>
+      <c r="F6" s="35">
+        <v>45567</v>
+      </c>
+      <c r="G6" s="12"/>
+    </row>
+    <row r="7" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="30"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="43"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="26"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="32">
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="26"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="11"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="26"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="11"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="24"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="11"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="24"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="11"/>
+    </row>
+    <row r="13" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="12"/>
+      <c r="D13" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="25"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="12"/>
+    </row>
+    <row r="14" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="31"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="44"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="24"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="11"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="11"/>
+      <c r="D16" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="24"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="11"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="11"/>
+      <c r="D17" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="24"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="11"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="11"/>
+      <c r="D18" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="24"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="11"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="D19" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="24"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="11"/>
+    </row>
+    <row r="20" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="12"/>
+      <c r="D20" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="25"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="12"/>
+    </row>
+    <row r="21" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="29"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="45"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="11"/>
+      <c r="D22" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" s="24"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="11"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="11"/>
+      <c r="D23" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="24"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="11"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="11"/>
+      <c r="D24" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" s="24"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="11"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="11"/>
+      <c r="D25" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25" s="24"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="11"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="11"/>
+      <c r="D26" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26" s="24"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="11"/>
+    </row>
+    <row r="27" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="12"/>
+      <c r="D27" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E27" s="25"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="12"/>
+    </row>
+    <row r="28" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E28" s="28">
         <v>45565</v>
       </c>
-      <c r="G4" s="33"/>
-      <c r="H4" s="42"/>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C5" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="24">
+      <c r="F28" s="40"/>
+      <c r="G28" s="46"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E29" s="24">
         <v>45565</v>
       </c>
-      <c r="G5" s="34">
-        <v>45565</v>
-      </c>
-      <c r="H5" s="11"/>
-    </row>
-    <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="25">
-        <v>45565</v>
-      </c>
-      <c r="G6" s="35"/>
-      <c r="H6" s="12"/>
-    </row>
-    <row r="7" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23" t="s">
+      <c r="F29" s="34"/>
+      <c r="G29" s="11"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="30"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="43"/>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C8" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="26"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="11"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C9" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="26"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="11"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C10" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" s="26"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="11"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C11" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="24"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="11"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C12" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="24"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="11"/>
-    </row>
-    <row r="13" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F13" s="25"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="12"/>
-    </row>
-    <row r="14" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="16" t="s">
+      <c r="E30" s="24">
+        <v>45567</v>
+      </c>
+      <c r="F30" s="34"/>
+      <c r="G30" s="11"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="F14" s="31"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="44"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C15" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F15" s="24"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="11"/>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C16" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F16" s="24"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="11"/>
-    </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C17" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="11"/>
-      <c r="E17" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F17" s="24"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="11"/>
-    </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C18" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="24"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="11"/>
-    </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C19" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="11"/>
-      <c r="E19" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F19" s="24"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="11"/>
-    </row>
-    <row r="20" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20" s="12"/>
-      <c r="E20" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F20" s="25"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="12"/>
-    </row>
-    <row r="21" spans="3:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="F21" s="29"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="45"/>
-    </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C22" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="11"/>
-      <c r="E22" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F22" s="24"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="11"/>
-    </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C23" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F23" s="24"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="11"/>
-    </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C24" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24" s="11"/>
-      <c r="E24" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F24" s="24"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="11"/>
-    </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C25" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D25" s="11"/>
-      <c r="E25" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F25" s="24"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="11"/>
-    </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C26" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D26" s="11"/>
-      <c r="E26" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F26" s="24"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="11"/>
-    </row>
-    <row r="27" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C27" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D27" s="12"/>
-      <c r="E27" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F27" s="25"/>
-      <c r="G27" s="35"/>
-      <c r="H27" s="12"/>
-    </row>
-    <row r="28" spans="3:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C28" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="F28" s="28">
-        <v>45565</v>
-      </c>
-      <c r="G28" s="40"/>
-      <c r="H28" s="46"/>
-    </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C29" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D29" s="11"/>
-      <c r="E29" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F29" s="24">
-        <v>45565</v>
-      </c>
-      <c r="G29" s="34"/>
-      <c r="H29" s="11"/>
-    </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C30" s="8" t="s">
+      <c r="C31" s="11"/>
+      <c r="D31" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31" s="24"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="11"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="11"/>
+      <c r="D32" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E32" s="24"/>
+      <c r="F32" s="34"/>
+      <c r="G32" s="11"/>
+    </row>
+    <row r="33" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D30" s="11"/>
-      <c r="E30" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F30" s="24"/>
-      <c r="G30" s="34"/>
-      <c r="H30" s="11"/>
-    </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C31" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D31" s="11"/>
-      <c r="E31" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F31" s="24"/>
-      <c r="G31" s="34"/>
-      <c r="H31" s="11"/>
-    </row>
-    <row r="32" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C32" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D32" s="11"/>
-      <c r="E32" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F32" s="24"/>
-      <c r="G32" s="34"/>
-      <c r="H32" s="11"/>
-    </row>
-    <row r="33" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C33" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D33" s="12"/>
-      <c r="E33" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F33" s="25"/>
-      <c r="G33" s="35"/>
-      <c r="H33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E33" s="25"/>
+      <c r="F33" s="35"/>
+      <c r="G33" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="E5:E6 E8:E13 E15:E20 E22:E27 E29:E1048576">
+  <conditionalFormatting sqref="D5:D6 D8:D13 D15:D20 D22:D27 D29:D1048576">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"V"</formula>
     </cfRule>

</xml_diff>

<commit_message>
update analyse des variables (conservation/exclusion)
</commit_message>
<xml_diff>
--- a/Admin/Dashboard_Appli_BI.xlsx
+++ b/Admin/Dashboard_Appli_BI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexi\Documents\files\Cours\Master\S9\UE_appli_bi\BanqueBI\Admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75792C0D-67E3-4EC9-987A-530C827C9ABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2ED1BEA-454D-4D8E-BF2C-82D1E73638CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="43">
   <si>
     <t>Tâches</t>
   </si>
@@ -147,10 +147,13 @@
     <t>Abdelghani</t>
   </si>
   <si>
-    <t>Python / Anaconda / VSC</t>
-  </si>
-  <si>
     <t>Alexis / Walid</t>
+  </si>
+  <si>
+    <t>Overleaf</t>
+  </si>
+  <si>
+    <t>Python / Anaconda / VSC / Word</t>
   </si>
 </sst>
 </file>
@@ -946,7 +949,7 @@
   <dimension ref="B1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1004,7 +1007,9 @@
       <c r="F4" s="33">
         <v>45567</v>
       </c>
-      <c r="G4" s="42"/>
+      <c r="G4" s="42" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
@@ -1022,7 +1027,9 @@
       <c r="F5" s="34">
         <v>45565</v>
       </c>
-      <c r="G5" s="11"/>
+      <c r="G5" s="11" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="9" t="s">
@@ -1040,7 +1047,9 @@
       <c r="F6" s="35">
         <v>45567</v>
       </c>
-      <c r="G6" s="12"/>
+      <c r="G6" s="12" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="7" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
@@ -1048,9 +1057,11 @@
       </c>
       <c r="C7" s="23"/>
       <c r="D7" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="30"/>
+        <v>34</v>
+      </c>
+      <c r="E7" s="30">
+        <v>45565</v>
+      </c>
       <c r="F7" s="36"/>
       <c r="G7" s="43"/>
     </row>
@@ -1071,7 +1082,7 @@
         <v>45569</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -1079,7 +1090,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>34</v>
@@ -1089,18 +1100,22 @@
       </c>
       <c r="F9" s="37"/>
       <c r="G9" s="11" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="13"/>
+      <c r="C10" s="13" t="s">
+        <v>39</v>
+      </c>
       <c r="D10" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="26"/>
+        <v>34</v>
+      </c>
+      <c r="E10" s="26">
+        <v>45571</v>
+      </c>
       <c r="F10" s="37"/>
       <c r="G10" s="11"/>
     </row>

</xml_diff>

<commit_message>
début config main principal + code livrable
</commit_message>
<xml_diff>
--- a/Admin/Dashboard_Appli_BI.xlsx
+++ b/Admin/Dashboard_Appli_BI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexi\Documents\files\Cours\Master\S9\UE_appli_bi\BanqueBI\Admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27501C29-EB2B-4EF3-BCA0-6F415F9043C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{602171EC-D742-47DA-95C0-85C457311D64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2246,7 +2246,7 @@
   <dimension ref="B1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2591,7 +2591,7 @@
         <v>33</v>
       </c>
       <c r="E22" s="24">
-        <v>45615</v>
+        <v>45617</v>
       </c>
       <c r="F22" s="33"/>
       <c r="G22" s="58"/>
@@ -2673,12 +2673,14 @@
         <v>46</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E27" s="25"/>
+        <v>33</v>
+      </c>
+      <c r="E27" s="25">
+        <v>45617</v>
+      </c>
       <c r="F27" s="34"/>
       <c r="G27" s="59"/>
     </row>
@@ -2708,7 +2710,7 @@
         <v>38</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E29" s="24">
         <v>45565</v>
@@ -2726,7 +2728,7 @@
         <v>38</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E30" s="24">
         <v>45567</v>

</xml_diff>

<commit_message>
last update code + diagrammes + images ressources
</commit_message>
<xml_diff>
--- a/Admin/Dashboard_Appli_BI.xlsx
+++ b/Admin/Dashboard_Appli_BI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexi\Documents\files\Cours\Master\S9\UE_appli_bi\BanqueBI\Admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{602171EC-D742-47DA-95C0-85C457311D64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B794CF1-36C8-4A5A-9F03-D5331E86CD42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{220A2BCB-677B-40EA-8392-4D244C57C13F}"/>
   </bookViews>
   <sheets>
     <sheet name="TASKS" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="51">
   <si>
     <t>Tâches</t>
   </si>
@@ -134,9 +134,6 @@
     <t>Résultats</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>EC</t>
   </si>
   <si>
@@ -183,6 +180,15 @@
   </si>
   <si>
     <t>Durée</t>
+  </si>
+  <si>
+    <t>Bonus</t>
+  </si>
+  <si>
+    <t>Dashboard BI</t>
+  </si>
+  <si>
+    <t>Python / Anaconda / VSC</t>
   </si>
 </sst>
 </file>
@@ -220,7 +226,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -263,8 +269,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="32">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -663,11 +675,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -798,18 +849,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -852,9 +891,6 @@
     <xf numFmtId="14" fontId="1" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="5" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -880,6 +916,63 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1044,9 +1137,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'DATA-GANTT'!$B$4:$B$13</c:f>
+              <c:f>'DATA-GANTT'!$B$4:$B$29</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>Description des données</c:v>
                 </c:pt>
@@ -1076,16 +1169,64 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Découpage</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Implémentation</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Script général</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1er Script - SVM</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2e Script - kNN</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3e Script - Naive Bayes</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4e Script - Autre</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Readme</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Rapport</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Présentation</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Données</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Méthodes de classification</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Résultats</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Conclusion</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Relecture</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Bonus</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Dashboard BI</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'DATA-GANTT'!$C$4:$C$13</c:f>
+              <c:f>'DATA-GANTT'!$C$4:$C$29</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>45565</c:v>
                 </c:pt>
@@ -1115,6 +1256,54 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>45598</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45599</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45617</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>45599</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>45599</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>45599</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>45599</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>45617</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>45565</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>45565</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>45567</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>45611</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>45615</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>45615</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>45633</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>45619</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>45619</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1161,6 +1350,44 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000008-C3A7-4C8E-B9EA-EBD10701F702}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-C3A7-4C8E-B9EA-EBD10701F702}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
             <c:idx val="3"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
@@ -1179,12 +1406,516 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000A-C3A7-4C8E-B9EA-EBD10701F702}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-C3A7-4C8E-B9EA-EBD10701F702}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000C-C3A7-4C8E-B9EA-EBD10701F702}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-C3A7-4C8E-B9EA-EBD10701F702}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000E-C3A7-4C8E-B9EA-EBD10701F702}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-C3A7-4C8E-B9EA-EBD10701F702}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-C3A7-4C8E-B9EA-EBD10701F702}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000010-C3A7-4C8E-B9EA-EBD10701F702}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-C3A7-4C8E-B9EA-EBD10701F702}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="13"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000012-C3A7-4C8E-B9EA-EBD10701F702}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="14"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-C3A7-4C8E-B9EA-EBD10701F702}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="15"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000014-C3A7-4C8E-B9EA-EBD10701F702}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="16"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-C3A7-4C8E-B9EA-EBD10701F702}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="17"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-C3A7-4C8E-B9EA-EBD10701F702}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="18"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000016-C3A7-4C8E-B9EA-EBD10701F702}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="19"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000017-C3A7-4C8E-B9EA-EBD10701F702}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="20"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000018-C3A7-4C8E-B9EA-EBD10701F702}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="21"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000019-C3A7-4C8E-B9EA-EBD10701F702}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="22"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001A-C3A7-4C8E-B9EA-EBD10701F702}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="23"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001B-C3A7-4C8E-B9EA-EBD10701F702}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="24"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-C3A7-4C8E-B9EA-EBD10701F702}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="25"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001C-C3A7-4C8E-B9EA-EBD10701F702}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>'DATA-GANTT'!$B$4:$B$29</c:f>
+              <c:strCache>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>Description des données</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Courte description des jeux de données</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Analyse des métriques des jeux de données</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Préparation des données</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Exploration</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Nettoyage</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Fusion</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Recodage</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Prétraitement</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Découpage</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Implémentation</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Script général</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1er Script - SVM</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2e Script - kNN</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3e Script - Naive Bayes</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4e Script - Autre</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Readme</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Rapport</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Présentation</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Données</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Méthodes de classification</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Résultats</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Conclusion</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Relecture</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Bonus</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Dashboard BI</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'DATA-GANTT'!$E$4:$E$13</c:f>
+              <c:f>'DATA-GANTT'!$E$4:$E$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -1213,6 +1944,54 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -2243,10 +3022,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:G34"/>
+  <dimension ref="B1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2285,7 +3064,7 @@
         <v>4</v>
       </c>
       <c r="G3" s="39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2293,10 +3072,10 @@
         <v>5</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E4" s="31">
         <v>45565</v>
@@ -2304,8 +3083,8 @@
       <c r="F4" s="32">
         <v>45567</v>
       </c>
-      <c r="G4" s="54" t="s">
-        <v>40</v>
+      <c r="G4" s="50" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
@@ -2313,10 +3092,10 @@
         <v>10</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E5" s="24">
         <v>45565</v>
@@ -2324,17 +3103,17 @@
       <c r="F5" s="33">
         <v>45565</v>
       </c>
-      <c r="G5" s="55"/>
+      <c r="G5" s="51"/>
     </row>
     <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="E6" s="25">
         <v>45565</v>
@@ -2342,17 +3121,17 @@
       <c r="F6" s="34">
         <v>45567</v>
       </c>
-      <c r="G6" s="56"/>
+      <c r="G6" s="52"/>
     </row>
     <row r="7" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7" s="30">
         <v>45565</v>
@@ -2360,8 +3139,8 @@
       <c r="F7" s="35">
         <v>45599</v>
       </c>
-      <c r="G7" s="51" t="s">
-        <v>41</v>
+      <c r="G7" s="47" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
@@ -2369,10 +3148,10 @@
         <v>11</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E8" s="26">
         <v>45565</v>
@@ -2380,17 +3159,17 @@
       <c r="F8" s="36">
         <v>45569</v>
       </c>
-      <c r="G8" s="52"/>
+      <c r="G8" s="48"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E9" s="26">
         <v>45566</v>
@@ -2398,17 +3177,17 @@
       <c r="F9" s="36">
         <v>45571</v>
       </c>
-      <c r="G9" s="52"/>
+      <c r="G9" s="48"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E10" s="26">
         <v>45571</v>
@@ -2416,17 +3195,17 @@
       <c r="F10" s="36">
         <v>45592</v>
       </c>
-      <c r="G10" s="52"/>
+      <c r="G10" s="48"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E11" s="24">
         <v>45596</v>
@@ -2434,17 +3213,17 @@
       <c r="F11" s="33">
         <v>45597</v>
       </c>
-      <c r="G11" s="52"/>
+      <c r="G11" s="48"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E12" s="24">
         <v>45597</v>
@@ -2452,17 +3231,17 @@
       <c r="F12" s="24">
         <v>45598</v>
       </c>
-      <c r="G12" s="52"/>
+      <c r="G12" s="48"/>
     </row>
     <row r="13" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E13" s="25">
         <v>45598</v>
@@ -2470,24 +3249,24 @@
       <c r="F13" s="34">
         <v>45599</v>
       </c>
-      <c r="G13" s="53"/>
+      <c r="G13" s="49"/>
     </row>
     <row r="14" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="16" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="48" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="63" t="s">
-        <v>47</v>
-      </c>
-      <c r="F14" s="64"/>
-      <c r="G14" s="69" t="s">
-        <v>47</v>
+        <v>43</v>
+      </c>
+      <c r="D14" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="59"/>
+      <c r="G14" s="64" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
@@ -2495,89 +3274,91 @@
         <v>17</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="49"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="66"/>
-      <c r="G15" s="70"/>
+        <v>43</v>
+      </c>
+      <c r="D15" s="45"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="61"/>
+      <c r="G15" s="65"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16" s="49"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="66"/>
-      <c r="G16" s="70"/>
+        <v>43</v>
+      </c>
+      <c r="D16" s="45"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="65"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="49"/>
-      <c r="E17" s="65"/>
-      <c r="F17" s="66"/>
-      <c r="G17" s="70"/>
+        <v>43</v>
+      </c>
+      <c r="D17" s="45"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="61"/>
+      <c r="G17" s="65"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" s="49"/>
-      <c r="E18" s="65"/>
-      <c r="F18" s="66"/>
-      <c r="G18" s="70"/>
+        <v>43</v>
+      </c>
+      <c r="D18" s="45"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="61"/>
+      <c r="G18" s="65"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="s">
         <v>21</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" s="49"/>
-      <c r="E19" s="65"/>
-      <c r="F19" s="66"/>
-      <c r="G19" s="70"/>
+        <v>43</v>
+      </c>
+      <c r="D19" s="45"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="61"/>
+      <c r="G19" s="65"/>
     </row>
     <row r="20" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="9" t="s">
         <v>22</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="50"/>
-      <c r="E20" s="67"/>
-      <c r="F20" s="68"/>
-      <c r="G20" s="71"/>
+        <v>43</v>
+      </c>
+      <c r="D20" s="46"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="63"/>
+      <c r="G20" s="66"/>
     </row>
     <row r="21" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E21" s="29">
         <v>45599</v>
       </c>
-      <c r="F21" s="37"/>
-      <c r="G21" s="57" t="s">
-        <v>41</v>
+      <c r="F21" s="37">
+        <v>45624</v>
+      </c>
+      <c r="G21" s="53" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
@@ -2585,26 +3366,28 @@
         <v>23</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E22" s="24">
         <v>45617</v>
       </c>
-      <c r="F22" s="33"/>
-      <c r="G22" s="58"/>
+      <c r="F22" s="33">
+        <v>45624</v>
+      </c>
+      <c r="G22" s="54"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E23" s="24">
         <v>45599</v>
@@ -2612,17 +3395,17 @@
       <c r="F23" s="33">
         <v>45605</v>
       </c>
-      <c r="G23" s="58"/>
+      <c r="G23" s="54"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E24" s="24">
         <v>45599</v>
@@ -2630,17 +3413,17 @@
       <c r="F24" s="33">
         <v>45600</v>
       </c>
-      <c r="G24" s="58"/>
+      <c r="G24" s="54"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E25" s="24">
         <v>45599</v>
@@ -2648,17 +3431,17 @@
       <c r="F25" s="33">
         <v>45608</v>
       </c>
-      <c r="G25" s="58"/>
+      <c r="G25" s="54"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="40" t="s">
         <v>27</v>
       </c>
       <c r="C26" s="41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E26" s="24">
         <v>45599</v>
@@ -2666,40 +3449,44 @@
       <c r="F26" s="33">
         <v>45608</v>
       </c>
-      <c r="G26" s="58"/>
+      <c r="G26" s="54"/>
     </row>
     <row r="27" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E27" s="25">
         <v>45617</v>
       </c>
-      <c r="F27" s="34"/>
-      <c r="G27" s="59"/>
+      <c r="F27" s="34">
+        <v>45624</v>
+      </c>
+      <c r="G27" s="55"/>
     </row>
     <row r="28" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="20" t="s">
         <v>9</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E28" s="28">
         <v>45565</v>
       </c>
-      <c r="F28" s="38"/>
-      <c r="G28" s="60" t="s">
-        <v>40</v>
+      <c r="F28" s="38">
+        <v>45634</v>
+      </c>
+      <c r="G28" s="56" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
@@ -2707,10 +3494,10 @@
         <v>28</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E29" s="24">
         <v>45565</v>
@@ -2718,17 +3505,17 @@
       <c r="F29" s="33">
         <v>45611</v>
       </c>
-      <c r="G29" s="61"/>
+      <c r="G29" s="57"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="8" t="s">
         <v>29</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E30" s="24">
         <v>45567</v>
@@ -2736,72 +3523,121 @@
       <c r="F30" s="33">
         <v>45611</v>
       </c>
-      <c r="G30" s="61"/>
+      <c r="G30" s="57"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E31" s="24">
         <v>45611</v>
       </c>
-      <c r="F31" s="33"/>
-      <c r="G31" s="61"/>
+      <c r="F31" s="33">
+        <v>45624</v>
+      </c>
+      <c r="G31" s="57"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E32" s="24">
         <v>45615</v>
       </c>
-      <c r="F32" s="33"/>
-      <c r="G32" s="61"/>
+      <c r="F32" s="33">
+        <v>45633</v>
+      </c>
+      <c r="G32" s="57"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="40" t="s">
         <v>30</v>
       </c>
       <c r="C33" s="41" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E33" s="42">
         <v>45615</v>
       </c>
-      <c r="F33" s="43"/>
-      <c r="G33" s="61"/>
+      <c r="F33" s="43">
+        <v>45633</v>
+      </c>
+      <c r="G33" s="57"/>
     </row>
     <row r="34" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C34" s="12" t="s">
+      <c r="B34" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="D34" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E34" s="25"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="62"/>
+      <c r="C34" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="D34" s="67" t="s">
+        <v>35</v>
+      </c>
+      <c r="E34" s="42">
+        <v>45633</v>
+      </c>
+      <c r="F34" s="43">
+        <v>45634</v>
+      </c>
+      <c r="G34" s="57"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="70" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35" s="71" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35" s="71" t="s">
+        <v>35</v>
+      </c>
+      <c r="E35" s="72">
+        <v>45619</v>
+      </c>
+      <c r="F35" s="72">
+        <v>45620</v>
+      </c>
+      <c r="G35" s="73" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E36" s="68">
+        <v>45619</v>
+      </c>
+      <c r="F36" s="68">
+        <v>45620</v>
+      </c>
+      <c r="G36" s="74"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="G35:G36"/>
     <mergeCell ref="D14:D20"/>
     <mergeCell ref="G7:G13"/>
     <mergeCell ref="G4:G6"/>
@@ -2811,7 +3647,7 @@
     <mergeCell ref="G14:G20"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="D5:D6 D8:D13 D22:D27 D29:D1048576">
+  <conditionalFormatting sqref="D5:D6 D8:D13 D22:D27 D29:D34 D36:D1048576">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"V"</formula>
     </cfRule>
@@ -2829,10 +3665,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2ACBA6B-9B44-45DB-BEB2-107A0E39573C}">
-  <dimension ref="B2:E27"/>
+  <dimension ref="B2:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2845,30 +3681,30 @@
   <sheetData>
     <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="44" t="s">
+      <c r="D3" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="39" t="s">
-        <v>48</v>
+      <c r="E3" s="77" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="31">
+      <c r="C4" s="69">
         <v>45565</v>
       </c>
-      <c r="D4" s="32">
+      <c r="D4" s="69">
         <v>45567</v>
       </c>
-      <c r="E4" s="45">
+      <c r="E4" s="78">
         <f>D4-C4</f>
         <v>2</v>
       </c>
@@ -2877,28 +3713,28 @@
       <c r="B5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="24">
+      <c r="C5" s="81">
         <v>45565</v>
       </c>
-      <c r="D5" s="33">
+      <c r="D5" s="81">
         <v>45566</v>
       </c>
-      <c r="E5" s="46">
-        <f t="shared" ref="E5:E23" si="0">D5-C5</f>
+      <c r="E5" s="79">
+        <f t="shared" ref="E5:E29" si="0">D5-C5</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="25">
+        <v>34</v>
+      </c>
+      <c r="C6" s="68">
         <v>45565</v>
       </c>
-      <c r="D6" s="34">
+      <c r="D6" s="68">
         <v>45567</v>
       </c>
-      <c r="E6" s="46">
+      <c r="E6" s="80">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -2907,58 +3743,58 @@
       <c r="B7" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="30">
+      <c r="C7" s="82">
         <v>45565</v>
       </c>
-      <c r="D7" s="35">
+      <c r="D7" s="82">
         <v>45599</v>
       </c>
-      <c r="E7" s="46">
+      <c r="E7" s="78">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="26">
+      <c r="C8" s="81">
         <v>45565</v>
       </c>
-      <c r="D8" s="36">
+      <c r="D8" s="81">
         <v>45569</v>
       </c>
-      <c r="E8" s="46">
+      <c r="E8" s="79">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="26">
+      <c r="C9" s="81">
         <v>45566</v>
       </c>
-      <c r="D9" s="36">
+      <c r="D9" s="81">
         <v>45571</v>
       </c>
-      <c r="E9" s="46">
+      <c r="E9" s="79">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="26">
+      <c r="C10" s="81">
         <v>45571</v>
       </c>
-      <c r="D10" s="36">
+      <c r="D10" s="81">
         <v>45592</v>
       </c>
-      <c r="E10" s="46">
+      <c r="E10" s="79">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
@@ -2967,13 +3803,13 @@
       <c r="B11" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="24">
+      <c r="C11" s="81">
         <v>45596</v>
       </c>
-      <c r="D11" s="33">
+      <c r="D11" s="81">
         <v>45599</v>
       </c>
-      <c r="E11" s="46">
+      <c r="E11" s="79">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -2982,13 +3818,13 @@
       <c r="B12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="24">
+      <c r="C12" s="81">
         <v>45598</v>
       </c>
-      <c r="D12" s="33">
+      <c r="D12" s="81">
         <v>45599</v>
       </c>
-      <c r="E12" s="46">
+      <c r="E12" s="79">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -2997,13 +3833,13 @@
       <c r="B13" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="25">
+      <c r="C13" s="68">
         <v>45598</v>
       </c>
-      <c r="D13" s="34">
+      <c r="D13" s="68">
         <v>45599</v>
       </c>
-      <c r="E13" s="46">
+      <c r="E13" s="80">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -3012,31 +3848,43 @@
       <c r="B14" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="29">
+      <c r="C14" s="83">
         <v>45599</v>
       </c>
-      <c r="D14" s="37"/>
-      <c r="E14" s="46"/>
+      <c r="D14" s="83">
+        <v>45624</v>
+      </c>
+      <c r="E14" s="78">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="46"/>
+      <c r="C15" s="81">
+        <v>45617</v>
+      </c>
+      <c r="D15" s="81">
+        <v>45624</v>
+      </c>
+      <c r="E15" s="79">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="24">
+      <c r="C16" s="81">
         <v>45599</v>
       </c>
-      <c r="D16" s="33">
+      <c r="D16" s="81">
         <v>45605</v>
       </c>
-      <c r="E16" s="46">
+      <c r="E16" s="79">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -3045,13 +3893,13 @@
       <c r="B17" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="24">
+      <c r="C17" s="81">
         <v>45599</v>
       </c>
-      <c r="D17" s="33">
+      <c r="D17" s="81">
         <v>45600</v>
       </c>
-      <c r="E17" s="46">
+      <c r="E17" s="79">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -3060,61 +3908,73 @@
       <c r="B18" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="24">
+      <c r="C18" s="81">
         <v>45599</v>
       </c>
-      <c r="D18" s="33">
+      <c r="D18" s="81">
         <v>45608</v>
       </c>
-      <c r="E18" s="46">
+      <c r="E18" s="79">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="40" t="s">
+      <c r="B19" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="24">
+      <c r="C19" s="81">
         <v>45599</v>
       </c>
-      <c r="D19" s="33">
+      <c r="D19" s="81">
         <v>45608</v>
       </c>
-      <c r="E19" s="46">
+      <c r="E19" s="79">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" s="25"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="46"/>
+        <v>45</v>
+      </c>
+      <c r="C20" s="68">
+        <v>45617</v>
+      </c>
+      <c r="D20" s="68">
+        <v>45624</v>
+      </c>
+      <c r="E20" s="80">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="28">
+      <c r="C21" s="84">
         <v>45565</v>
       </c>
-      <c r="D21" s="38"/>
-      <c r="E21" s="46"/>
+      <c r="D21" s="84">
+        <v>45634</v>
+      </c>
+      <c r="E21" s="78">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="24">
+      <c r="C22" s="81">
         <v>45565</v>
       </c>
-      <c r="D22" s="33">
+      <c r="D22" s="81">
         <v>45611</v>
       </c>
-      <c r="E22" s="46">
+      <c r="E22" s="79">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
@@ -3123,13 +3983,13 @@
       <c r="B23" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="24">
+      <c r="C23" s="81">
         <v>45567</v>
       </c>
-      <c r="D23" s="33">
+      <c r="D23" s="81">
         <v>45611</v>
       </c>
-      <c r="E23" s="46">
+      <c r="E23" s="79">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
@@ -3138,39 +3998,91 @@
       <c r="B24" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="24">
+      <c r="C24" s="81">
         <v>45611</v>
       </c>
-      <c r="D24" s="33"/>
-      <c r="E24" s="46"/>
+      <c r="D24" s="81">
+        <v>45624</v>
+      </c>
+      <c r="E24" s="79">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="24">
+      <c r="C25" s="81">
         <v>45615</v>
       </c>
-      <c r="D25" s="33"/>
-      <c r="E25" s="46"/>
+      <c r="D25" s="81">
+        <v>45633</v>
+      </c>
+      <c r="E25" s="79">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="40" t="s">
+      <c r="B26" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="42">
+      <c r="C26" s="85">
         <v>45615</v>
       </c>
-      <c r="D26" s="43"/>
-      <c r="E26" s="46"/>
+      <c r="D26" s="85">
+        <v>45633</v>
+      </c>
+      <c r="E26" s="79">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
     </row>
     <row r="27" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C27" s="25"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="47"/>
+        <v>44</v>
+      </c>
+      <c r="C27" s="85">
+        <v>45633</v>
+      </c>
+      <c r="D27" s="85">
+        <v>45634</v>
+      </c>
+      <c r="E27" s="80">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="70" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="72">
+        <v>45619</v>
+      </c>
+      <c r="D28" s="72">
+        <v>45620</v>
+      </c>
+      <c r="E28" s="78">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="68">
+        <v>45619</v>
+      </c>
+      <c r="D29" s="68">
+        <v>45620</v>
+      </c>
+      <c r="E29" s="80">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3182,9 +4094,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1366EFC5-598A-4BD5-8B86-30AF96D19E22}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W20" sqref="W20"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>